<commit_message>
Intially proposed WireFrames (#12)
</commit_message>
<xml_diff>
--- a/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
+++ b/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJSU\NEW_SEM\202\Project\fa20-cmpe-202-sec-02-team-project-team_3\SCRUM_Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62043FF0-4E8D-4BBA-8010-17706E802968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8592FE25-1873-49BD-9B29-2A9B57088324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
-    <sheet name="Burndown" sheetId="2" r:id="rId2"/>
+    <sheet name="Overall_Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -616,28 +616,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -648,10 +633,25 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,7 +1995,9 @@
   </sheetPr>
   <dimension ref="A1:BW1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2010,108 +2012,108 @@
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="50"/>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
       <c r="R1" s="50"/>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
       <c r="Y1" s="50"/>
-      <c r="Z1" s="48" t="s">
+      <c r="Z1" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="49" t="s">
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
-      <c r="AK1" s="43"/>
-      <c r="AL1" s="43"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
       <c r="AM1" s="50"/>
-      <c r="AN1" s="48" t="s">
+      <c r="AN1" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AQ1" s="43"/>
-      <c r="AR1" s="43"/>
-      <c r="AS1" s="43"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="49" t="s">
+      <c r="AO1" s="49"/>
+      <c r="AP1" s="49"/>
+      <c r="AQ1" s="49"/>
+      <c r="AR1" s="49"/>
+      <c r="AS1" s="49"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="AV1" s="43"/>
-      <c r="AW1" s="43"/>
-      <c r="AX1" s="43"/>
-      <c r="AY1" s="43"/>
-      <c r="AZ1" s="43"/>
+      <c r="AV1" s="49"/>
+      <c r="AW1" s="49"/>
+      <c r="AX1" s="49"/>
+      <c r="AY1" s="49"/>
+      <c r="AZ1" s="49"/>
       <c r="BA1" s="50"/>
-      <c r="BB1" s="48" t="s">
+      <c r="BB1" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="BC1" s="43"/>
-      <c r="BD1" s="43"/>
-      <c r="BE1" s="43"/>
-      <c r="BF1" s="43"/>
-      <c r="BG1" s="43"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="49" t="s">
+      <c r="BC1" s="49"/>
+      <c r="BD1" s="49"/>
+      <c r="BE1" s="49"/>
+      <c r="BF1" s="49"/>
+      <c r="BG1" s="49"/>
+      <c r="BH1" s="54"/>
+      <c r="BI1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="BJ1" s="43"/>
-      <c r="BK1" s="43"/>
-      <c r="BL1" s="43"/>
-      <c r="BM1" s="43"/>
-      <c r="BN1" s="43"/>
+      <c r="BJ1" s="49"/>
+      <c r="BK1" s="49"/>
+      <c r="BL1" s="49"/>
+      <c r="BM1" s="49"/>
+      <c r="BN1" s="49"/>
       <c r="BO1" s="50"/>
-      <c r="BP1" s="42" t="s">
+      <c r="BP1" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="BQ1" s="43"/>
-      <c r="BR1" s="43"/>
-      <c r="BS1" s="43"/>
-      <c r="BT1" s="43"/>
-      <c r="BU1" s="43"/>
-      <c r="BV1" s="44"/>
+      <c r="BQ1" s="49"/>
+      <c r="BR1" s="49"/>
+      <c r="BS1" s="49"/>
+      <c r="BT1" s="49"/>
+      <c r="BU1" s="49"/>
+      <c r="BV1" s="54"/>
     </row>
     <row r="2" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2326,10 +2328,10 @@
       </c>
     </row>
     <row r="3" spans="1:75" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="7">
         <v>44101</v>
       </c>
@@ -2543,9 +2545,9 @@
       <c r="BW3" s="9"/>
     </row>
     <row r="4" spans="1:75" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11">
         <v>160</v>
@@ -2831,9 +2833,9 @@
       </c>
     </row>
     <row r="5" spans="1:75" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="10">
         <v>160</v>
       </c>
@@ -2954,7 +2956,7 @@
       </c>
     </row>
     <row r="6" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="55" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -3046,7 +3048,7 @@
       <c r="BV6" s="30"/>
     </row>
     <row r="7" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="15" t="s">
         <v>39</v>
       </c>
@@ -3132,7 +3134,7 @@
       <c r="BV7" s="30"/>
     </row>
     <row r="8" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3222,7 +3224,7 @@
       <c r="BV8" s="30"/>
     </row>
     <row r="9" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
@@ -3308,7 +3310,7 @@
       <c r="BV9" s="30"/>
     </row>
     <row r="10" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
@@ -3392,7 +3394,7 @@
       <c r="BV10" s="30"/>
     </row>
     <row r="11" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="40" t="s">
         <v>49</v>
       </c>
@@ -3478,7 +3480,7 @@
       <c r="BV11" s="30"/>
     </row>
     <row r="12" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="40" t="s">
         <v>50</v>
       </c>
@@ -3560,7 +3562,7 @@
       <c r="BV12" s="30"/>
     </row>
     <row r="13" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="15"/>
@@ -3642,7 +3644,7 @@
       <c r="BV13" s="30"/>
     </row>
     <row r="14" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="15"/>
       <c r="C14" s="41" t="s">
         <v>42</v>
@@ -3722,7 +3724,7 @@
       <c r="BV14" s="30"/>
     </row>
     <row r="15" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17">
@@ -3800,7 +3802,7 @@
       <c r="BV15" s="30"/>
     </row>
     <row r="16" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="42" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="15"/>
@@ -3882,7 +3884,7 @@
       <c r="BV16" s="30"/>
     </row>
     <row r="17" spans="1:74" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="15"/>
       <c r="C17" s="41" t="s">
         <v>36</v>
@@ -3962,7 +3964,7 @@
       <c r="BV17" s="30"/>
     </row>
     <row r="18" spans="1:74" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="15"/>
       <c r="C18" s="41" t="s">
         <v>38</v>
@@ -29748,12 +29750,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="D2:D3"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="A13:A15"/>
@@ -29765,6 +29761,12 @@
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="S1:Y1"/>
     <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -29778,8 +29780,8 @@
   </sheetPr>
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Frontend Modules Login Sign Up and Admin
</commit_message>
<xml_diff>
--- a/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
+++ b/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJSU\NEW_SEM\202\Project\fa20-cmpe-202-sec-02-team-project-team_3\SCRUM_Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1A958B-96D0-4C86-B9E7-C7918FF19D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAA90EB-A7AE-49A3-A0CB-6A16C37ED63F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,24 +803,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,6 +836,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2371,7 +2371,9 @@
   </sheetPr>
   <dimension ref="A1:BX1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2388,109 +2390,109 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="58" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="59" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="58" t="s">
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="59" t="s">
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="58" t="s">
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="59" t="s">
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="AW1" s="53"/>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
-      <c r="AZ1" s="53"/>
-      <c r="BA1" s="53"/>
-      <c r="BB1" s="60"/>
-      <c r="BC1" s="58" t="s">
+      <c r="AW1" s="47"/>
+      <c r="AX1" s="47"/>
+      <c r="AY1" s="47"/>
+      <c r="AZ1" s="47"/>
+      <c r="BA1" s="47"/>
+      <c r="BB1" s="54"/>
+      <c r="BC1" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="53"/>
-      <c r="BE1" s="53"/>
-      <c r="BF1" s="53"/>
-      <c r="BG1" s="53"/>
-      <c r="BH1" s="53"/>
-      <c r="BI1" s="54"/>
-      <c r="BJ1" s="59" t="s">
+      <c r="BD1" s="47"/>
+      <c r="BE1" s="47"/>
+      <c r="BF1" s="47"/>
+      <c r="BG1" s="47"/>
+      <c r="BH1" s="47"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="53"/>
-      <c r="BL1" s="53"/>
-      <c r="BM1" s="53"/>
-      <c r="BN1" s="53"/>
-      <c r="BO1" s="53"/>
-      <c r="BP1" s="60"/>
-      <c r="BQ1" s="52" t="s">
+      <c r="BK1" s="47"/>
+      <c r="BL1" s="47"/>
+      <c r="BM1" s="47"/>
+      <c r="BN1" s="47"/>
+      <c r="BO1" s="47"/>
+      <c r="BP1" s="54"/>
+      <c r="BQ1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="BR1" s="53"/>
-      <c r="BS1" s="53"/>
-      <c r="BT1" s="53"/>
-      <c r="BU1" s="53"/>
-      <c r="BV1" s="53"/>
-      <c r="BW1" s="54"/>
+      <c r="BR1" s="47"/>
+      <c r="BS1" s="47"/>
+      <c r="BT1" s="47"/>
+      <c r="BU1" s="47"/>
+      <c r="BV1" s="47"/>
+      <c r="BW1" s="48"/>
     </row>
     <row r="2" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="41"/>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="59" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -2705,11 +2707,11 @@
       </c>
     </row>
     <row r="3" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="42"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="66"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="60"/>
       <c r="F3" s="7">
         <v>44101</v>
       </c>
@@ -2923,10 +2925,10 @@
       <c r="BX3" s="9"/>
     </row>
     <row r="4" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="62"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11">
         <v>160</v>
@@ -3212,10 +3214,10 @@
       </c>
     </row>
     <row r="5" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="63"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10">
         <f>SUM(E6:E46)</f>
         <v>160</v>
@@ -3505,7 +3507,7 @@
       </c>
     </row>
     <row r="6" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="49" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="44" t="s">
@@ -3592,7 +3594,7 @@
       <c r="BW6" s="29"/>
     </row>
     <row r="7" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="44" t="s">
         <v>38</v>
       </c>
@@ -3679,7 +3681,7 @@
       <c r="BW7" s="29"/>
     </row>
     <row r="8" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="44" t="s">
         <v>36</v>
       </c>
@@ -3764,7 +3766,7 @@
       <c r="BW8" s="29"/>
     </row>
     <row r="9" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="44" t="s">
         <v>61</v>
       </c>
@@ -3855,7 +3857,7 @@
       <c r="BW9" s="29"/>
     </row>
     <row r="10" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="44" t="s">
         <v>39</v>
       </c>
@@ -3944,7 +3946,7 @@
       <c r="BW10" s="29"/>
     </row>
     <row r="11" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="45" t="s">
         <v>46</v>
       </c>
@@ -4031,7 +4033,7 @@
       <c r="BW11" s="29"/>
     </row>
     <row r="12" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="45" t="s">
         <v>60</v>
       </c>
@@ -4122,7 +4124,7 @@
       <c r="BW12" s="29"/>
     </row>
     <row r="13" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="45" t="s">
         <v>62</v>
       </c>
@@ -4213,7 +4215,7 @@
       <c r="BW13" s="29"/>
     </row>
     <row r="14" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="45" t="s">
         <v>104</v>
       </c>
@@ -4298,7 +4300,7 @@
       <c r="BW14" s="29"/>
     </row>
     <row r="15" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="64" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -4387,7 +4389,7 @@
       <c r="BW15" s="29"/>
     </row>
     <row r="16" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="14" t="s">
         <v>64</v>
       </c>
@@ -4476,7 +4478,7 @@
       <c r="BW16" s="29"/>
     </row>
     <row r="17" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="14" t="s">
         <v>65</v>
       </c>
@@ -4565,7 +4567,7 @@
       <c r="BW17" s="29"/>
     </row>
     <row r="18" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="14" t="s">
         <v>66</v>
       </c>
@@ -4654,7 +4656,7 @@
       <c r="BW18" s="29"/>
     </row>
     <row r="19" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="61" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="44" t="s">
@@ -4745,7 +4747,7 @@
       <c r="BW19" s="29"/>
     </row>
     <row r="20" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="44" t="s">
         <v>71</v>
       </c>
@@ -4834,7 +4836,7 @@
       <c r="BW20" s="29"/>
     </row>
     <row r="21" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="63" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -4925,7 +4927,7 @@
       <c r="BW21" s="29"/>
     </row>
     <row r="22" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="14" t="s">
         <v>81</v>
       </c>
@@ -5014,7 +5016,7 @@
       <c r="BW22" s="29"/>
     </row>
     <row r="23" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="14" t="s">
         <v>82</v>
       </c>
@@ -5103,7 +5105,7 @@
       <c r="BW23" s="29"/>
     </row>
     <row r="24" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="14" t="s">
         <v>83</v>
       </c>
@@ -5192,7 +5194,7 @@
       </c>
     </row>
     <row r="25" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="39" t="s">
         <v>85</v>
       </c>
@@ -5281,7 +5283,7 @@
       <c r="BW25" s="29"/>
     </row>
     <row r="26" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="39" t="s">
         <v>86</v>
       </c>
@@ -5370,7 +5372,7 @@
       <c r="BW26" s="29"/>
     </row>
     <row r="27" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="39" t="s">
         <v>87</v>
       </c>
@@ -5459,7 +5461,7 @@
       <c r="BW27" s="29"/>
     </row>
     <row r="28" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="39" t="s">
         <v>88</v>
       </c>
@@ -5548,7 +5550,7 @@
       <c r="BW28" s="29"/>
     </row>
     <row r="29" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="66" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -5639,7 +5641,7 @@
       <c r="BW29" s="29"/>
     </row>
     <row r="30" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="39" t="s">
         <v>90</v>
       </c>
@@ -5728,7 +5730,7 @@
       <c r="BW30" s="29"/>
     </row>
     <row r="31" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="39" t="s">
         <v>91</v>
       </c>
@@ -5815,7 +5817,7 @@
       <c r="BW31" s="29"/>
     </row>
     <row r="32" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="39" t="s">
         <v>92</v>
       </c>
@@ -5906,7 +5908,7 @@
       <c r="BW32" s="29"/>
     </row>
     <row r="33" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="39" t="s">
         <v>93</v>
       </c>
@@ -5995,7 +5997,7 @@
       <c r="BW33" s="29"/>
     </row>
     <row r="34" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="39" t="s">
         <v>94</v>
       </c>
@@ -6084,7 +6086,7 @@
       <c r="BW34" s="29"/>
     </row>
     <row r="35" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="39" t="s">
         <v>95</v>
       </c>
@@ -6173,7 +6175,7 @@
       <c r="BW35" s="29"/>
     </row>
     <row r="36" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="39" t="s">
         <v>96</v>
       </c>
@@ -6262,7 +6264,7 @@
       <c r="BW36" s="29"/>
     </row>
     <row r="37" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="39" t="s">
         <v>97</v>
       </c>
@@ -6351,7 +6353,7 @@
       <c r="BW37" s="29"/>
     </row>
     <row r="38" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="39" t="s">
         <v>98</v>
       </c>
@@ -6442,7 +6444,7 @@
       <c r="BW38" s="29"/>
     </row>
     <row r="39" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="39" t="s">
         <v>99</v>
       </c>
@@ -6531,7 +6533,7 @@
       <c r="BW39" s="29"/>
     </row>
     <row r="40" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="39" t="s">
         <v>100</v>
       </c>
@@ -6620,7 +6622,7 @@
       <c r="BW40" s="29"/>
     </row>
     <row r="41" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="66" t="s">
         <v>73</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -6713,7 +6715,7 @@
       <c r="BW41" s="29"/>
     </row>
     <row r="42" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="14" t="s">
         <v>75</v>
       </c>
@@ -6804,7 +6806,7 @@
       <c r="BW42" s="29"/>
     </row>
     <row r="43" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="14" t="s">
         <v>76</v>
       </c>
@@ -6893,7 +6895,7 @@
       <c r="BW43" s="29"/>
     </row>
     <row r="44" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="14" t="s">
         <v>77</v>
       </c>
@@ -6984,7 +6986,7 @@
       <c r="BW44" s="29"/>
     </row>
     <row r="45" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="14" t="s">
         <v>78</v>
       </c>
@@ -7075,7 +7077,7 @@
       <c r="BW45" s="29"/>
     </row>
     <row r="46" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="14" t="s">
         <v>79</v>
       </c>
@@ -32879,6 +32881,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="A29:A40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="BQ1:BW1"/>
     <mergeCell ref="A6:A14"/>
     <mergeCell ref="AO1:AU1"/>
@@ -32894,11 +32901,6 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="A29:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Journal Update and small corrections
</commit_message>
<xml_diff>
--- a/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
+++ b/SCRUM_Sheet/Team3_SCRUM_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJSU\NEW_SEM\202\Project\fa20-cmpe-202-sec-02-team-project-team_3\SCRUM_Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EBF6DD-25BB-4202-AD0D-321A4E707B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6193D541-0B44-4E4A-8793-0E738B9D9143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -709,6 +709,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -818,6 +833,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -851,25 +884,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1720,127 +1735,127 @@
                   <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>98</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>98</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>98</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>78</c:v>
-                </c:pt>
                 <c:pt idx="37">
-                  <c:v>72</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>70</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>70</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>65</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>65</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>65</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>63</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>57</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>52</c:v>
+                <c:pt idx="47">
+                  <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>46</c:v>
-                </c:pt>
                 <c:pt idx="49">
-                  <c:v>46</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="57">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="61">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="60">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="62">
-                  <c:v>15</c:v>
-                </c:pt>
                 <c:pt idx="63">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>2</c:v>
@@ -2406,109 +2421,109 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="52" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="53" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="52" t="s">
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="53" t="s">
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="52" t="s">
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="47"/>
-      <c r="AT1" s="47"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="53" t="s">
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="AW1" s="47"/>
-      <c r="AX1" s="47"/>
-      <c r="AY1" s="47"/>
-      <c r="AZ1" s="47"/>
-      <c r="BA1" s="47"/>
-      <c r="BB1" s="54"/>
-      <c r="BC1" s="52" t="s">
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="53"/>
+      <c r="BB1" s="60"/>
+      <c r="BC1" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="47"/>
-      <c r="BE1" s="47"/>
-      <c r="BF1" s="47"/>
-      <c r="BG1" s="47"/>
-      <c r="BH1" s="47"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="53" t="s">
+      <c r="BD1" s="53"/>
+      <c r="BE1" s="53"/>
+      <c r="BF1" s="53"/>
+      <c r="BG1" s="53"/>
+      <c r="BH1" s="53"/>
+      <c r="BI1" s="54"/>
+      <c r="BJ1" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="47"/>
-      <c r="BL1" s="47"/>
-      <c r="BM1" s="47"/>
-      <c r="BN1" s="47"/>
-      <c r="BO1" s="47"/>
-      <c r="BP1" s="54"/>
-      <c r="BQ1" s="46" t="s">
+      <c r="BK1" s="53"/>
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="60"/>
+      <c r="BQ1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="BR1" s="47"/>
-      <c r="BS1" s="47"/>
-      <c r="BT1" s="47"/>
-      <c r="BU1" s="47"/>
-      <c r="BV1" s="47"/>
-      <c r="BW1" s="48"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="54"/>
     </row>
     <row r="2" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="61" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="41"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="65" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -2723,11 +2738,11 @@
       </c>
     </row>
     <row r="3" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="42"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="60"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="66"/>
       <c r="F3" s="7">
         <v>44101</v>
       </c>
@@ -2941,10 +2956,10 @@
       <c r="BX3" s="9"/>
     </row>
     <row r="4" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="56"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11">
         <v>160</v>
@@ -3230,10 +3245,10 @@
       </c>
     </row>
     <row r="5" spans="1:76" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="57"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10">
         <f>SUM(E6:E48)</f>
         <v>160</v>
@@ -3348,167 +3363,167 @@
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" ref="AH5" si="4">AG5 - SUM(AH6:AH48)</f>
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AI5" s="12">
         <f t="shared" ref="AI5" si="5">AH5 - SUM(AI6:AI48)</f>
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ref="AJ5" si="6">AI5 - SUM(AJ6:AJ48)</f>
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AK5" s="12">
         <f t="shared" ref="AK5" si="7">AJ5 - SUM(AK6:AK48)</f>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="AL5" s="12">
         <f t="shared" ref="AL5" si="8">AK5 - SUM(AL6:AL48)</f>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AM5" s="12">
         <f t="shared" ref="AM5" si="9">AL5 - SUM(AM6:AM48)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AN5" s="12">
         <f t="shared" ref="AN5" si="10">AM5 - SUM(AN6:AN48)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AO5" s="12">
         <f t="shared" ref="AO5" si="11">AN5 - SUM(AO6:AO48)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AP5" s="12">
         <f t="shared" ref="AP5" si="12">AO5 - SUM(AP6:AP48)</f>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ref="AQ5" si="13">AP5 - SUM(AQ6:AQ48)</f>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AR5" s="12">
         <f t="shared" ref="AR5" si="14">AQ5 - SUM(AR6:AR48)</f>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AS5" s="12">
         <f t="shared" ref="AS5" si="15">AR5 - SUM(AS6:AS48)</f>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AT5" s="12">
         <f t="shared" ref="AT5" si="16">AS5 - SUM(AT6:AT48)</f>
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AU5" s="12">
         <f t="shared" ref="AU5" si="17">AT5 - SUM(AU6:AU48)</f>
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV5" s="12">
         <f t="shared" ref="AV5" si="18">AU5 - SUM(AV6:AV48)</f>
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AW5" s="12">
         <f t="shared" ref="AW5" si="19">AV5 - SUM(AW6:AW48)</f>
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ref="AX5" si="20">AW5 - SUM(AX6:AX48)</f>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AY5" s="12">
         <f t="shared" ref="AY5" si="21">AX5 - SUM(AY6:AY48)</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AZ5" s="12">
         <f t="shared" ref="AZ5" si="22">AY5 - SUM(AZ6:AZ48)</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="BA5" s="12">
         <f t="shared" ref="BA5" si="23">AZ5 - SUM(BA6:BA48)</f>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="BB5" s="12">
         <f t="shared" ref="BB5" si="24">BA5 - SUM(BB6:BB48)</f>
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="BC5" s="12">
         <f t="shared" ref="BC5" si="25">BB5 - SUM(BC6:BC48)</f>
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="BD5" s="12">
         <f t="shared" ref="BD5" si="26">BC5 - SUM(BD6:BD48)</f>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ref="BE5" si="27">BD5 - SUM(BE6:BE48)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="BF5" s="12">
         <f t="shared" ref="BF5" si="28">BE5 - SUM(BF6:BF48)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="BG5" s="12">
         <f t="shared" ref="BG5" si="29">BF5 - SUM(BG6:BG48)</f>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="BH5" s="12">
         <f t="shared" ref="BH5" si="30">BG5 - SUM(BH6:BH48)</f>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="BI5" s="12">
         <f t="shared" ref="BI5" si="31">BH5 - SUM(BI6:BI48)</f>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="BJ5" s="12">
         <f t="shared" ref="BJ5" si="32">BI5 - SUM(BJ6:BJ48)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BK5" s="12">
         <f t="shared" ref="BK5" si="33">BJ5 - SUM(BK6:BK48)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ref="BL5" si="34">BK5 - SUM(BL6:BL48)</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="BM5" s="12">
         <f t="shared" ref="BM5" si="35">BL5 - SUM(BM6:BM48)</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="BN5" s="12">
         <f t="shared" ref="BN5" si="36">BM5 - SUM(BN6:BN48)</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="BO5" s="12">
         <f t="shared" ref="BO5" si="37">BN5 - SUM(BO6:BO48)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="BP5" s="12">
         <f t="shared" ref="BP5" si="38">BO5 - SUM(BP6:BP48)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="BQ5" s="12">
         <f t="shared" ref="BQ5" si="39">BP5 - SUM(BQ6:BQ48)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="BR5" s="12">
         <f t="shared" ref="BR5" si="40">BQ5 - SUM(BR6:BR48)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BS5" s="12">
         <f t="shared" ref="BS5" si="41">BR5 - SUM(BS6:BS48)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BT5" s="12">
         <f t="shared" ref="BT5" si="42">BS5 - SUM(BT6:BT48)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BU5" s="12">
         <f t="shared" ref="BU5" si="43">BT5 - SUM(BU6:BU48)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BV5" s="12">
         <f t="shared" ref="BV5" si="44">BU5 - SUM(BV6:BV48)</f>
@@ -3523,7 +3538,7 @@
       </c>
     </row>
     <row r="6" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="55" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="44" t="s">
@@ -3610,7 +3625,7 @@
       <c r="BW6" s="29"/>
     </row>
     <row r="7" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="44" t="s">
         <v>38</v>
       </c>
@@ -3697,7 +3712,7 @@
       <c r="BW7" s="29"/>
     </row>
     <row r="8" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="44" t="s">
         <v>36</v>
       </c>
@@ -3782,7 +3797,7 @@
       <c r="BW8" s="29"/>
     </row>
     <row r="9" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="44" t="s">
         <v>61</v>
       </c>
@@ -3873,7 +3888,7 @@
       <c r="BW9" s="29"/>
     </row>
     <row r="10" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="44" t="s">
         <v>39</v>
       </c>
@@ -3962,7 +3977,7 @@
       <c r="BW10" s="29"/>
     </row>
     <row r="11" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="45" t="s">
         <v>46</v>
       </c>
@@ -4049,7 +4064,7 @@
       <c r="BW11" s="29"/>
     </row>
     <row r="12" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="45" t="s">
         <v>60</v>
       </c>
@@ -4140,7 +4155,7 @@
       <c r="BW12" s="29"/>
     </row>
     <row r="13" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="45" t="s">
         <v>62</v>
       </c>
@@ -4231,7 +4246,7 @@
       <c r="BW13" s="29"/>
     </row>
     <row r="14" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="45" t="s">
         <v>105</v>
       </c>
@@ -4322,7 +4337,7 @@
       <c r="BW14" s="29"/>
     </row>
     <row r="15" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="45" t="s">
         <v>104</v>
       </c>
@@ -4407,7 +4422,7 @@
       <c r="BW15" s="29"/>
     </row>
     <row r="16" spans="1:76" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="49" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -4496,7 +4511,7 @@
       <c r="BW16" s="29"/>
     </row>
     <row r="17" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="14" t="s">
         <v>64</v>
       </c>
@@ -4585,7 +4600,7 @@
       <c r="BW17" s="29"/>
     </row>
     <row r="18" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="14" t="s">
         <v>65</v>
       </c>
@@ -4674,7 +4689,7 @@
       <c r="BW18" s="29"/>
     </row>
     <row r="19" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="14" t="s">
         <v>66</v>
       </c>
@@ -4763,7 +4778,7 @@
       <c r="BW19" s="29"/>
     </row>
     <row r="20" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="46" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="44" t="s">
@@ -4854,7 +4869,7 @@
       <c r="BW20" s="29"/>
     </row>
     <row r="21" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="44" t="s">
         <v>71</v>
       </c>
@@ -4943,7 +4958,7 @@
       <c r="BW21" s="29"/>
     </row>
     <row r="22" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="48" t="s">
         <v>84</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -5034,7 +5049,7 @@
       <c r="BW22" s="29"/>
     </row>
     <row r="23" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="14" t="s">
         <v>81</v>
       </c>
@@ -5123,7 +5138,7 @@
       <c r="BW23" s="29"/>
     </row>
     <row r="24" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="14" t="s">
         <v>82</v>
       </c>
@@ -5212,7 +5227,7 @@
       <c r="BW24" s="29"/>
     </row>
     <row r="25" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="14" t="s">
         <v>83</v>
       </c>
@@ -5301,7 +5316,7 @@
       </c>
     </row>
     <row r="26" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="39" t="s">
         <v>85</v>
       </c>
@@ -5390,7 +5405,7 @@
       <c r="BW26" s="29"/>
     </row>
     <row r="27" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="39" t="s">
         <v>86</v>
       </c>
@@ -5479,7 +5494,7 @@
       <c r="BW27" s="29"/>
     </row>
     <row r="28" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="39" t="s">
         <v>87</v>
       </c>
@@ -5568,7 +5583,7 @@
       <c r="BW28" s="29"/>
     </row>
     <row r="29" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="39" t="s">
         <v>88</v>
       </c>
@@ -5657,7 +5672,7 @@
       <c r="BW29" s="29"/>
     </row>
     <row r="30" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="51" t="s">
         <v>101</v>
       </c>
       <c r="B30" s="39" t="s">
@@ -5748,7 +5763,7 @@
       <c r="BW30" s="29"/>
     </row>
     <row r="31" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="39" t="s">
         <v>90</v>
       </c>
@@ -5837,7 +5852,7 @@
       <c r="BW31" s="29"/>
     </row>
     <row r="32" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="39" t="s">
         <v>91</v>
       </c>
@@ -5926,7 +5941,7 @@
       <c r="BW32" s="29"/>
     </row>
     <row r="33" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="39" t="s">
         <v>92</v>
       </c>
@@ -6013,7 +6028,7 @@
       <c r="BW33" s="29"/>
     </row>
     <row r="34" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="64"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="39" t="s">
         <v>93</v>
       </c>
@@ -6102,7 +6117,7 @@
       <c r="BW34" s="29"/>
     </row>
     <row r="35" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="39" t="s">
         <v>94</v>
       </c>
@@ -6191,7 +6206,7 @@
       <c r="BW35" s="29"/>
     </row>
     <row r="36" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="39" t="s">
         <v>95</v>
       </c>
@@ -6280,7 +6295,7 @@
       <c r="BW36" s="29"/>
     </row>
     <row r="37" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="39" t="s">
         <v>96</v>
       </c>
@@ -6369,7 +6384,7 @@
       <c r="BW37" s="29"/>
     </row>
     <row r="38" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="39" t="s">
         <v>97</v>
       </c>
@@ -6456,7 +6471,7 @@
       <c r="BW38" s="29"/>
     </row>
     <row r="39" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="64"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="39" t="s">
         <v>98</v>
       </c>
@@ -6545,7 +6560,7 @@
       <c r="BW39" s="29"/>
     </row>
     <row r="40" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="64"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="39" t="s">
         <v>99</v>
       </c>
@@ -6634,7 +6649,7 @@
       <c r="BW40" s="29"/>
     </row>
     <row r="41" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="65"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="39" t="s">
         <v>100</v>
       </c>
@@ -6723,7 +6738,7 @@
       <c r="BW41" s="29"/>
     </row>
     <row r="42" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="51" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -6814,7 +6829,7 @@
       <c r="BW42" s="29"/>
     </row>
     <row r="43" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="64"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="14" t="s">
         <v>75</v>
       </c>
@@ -6903,7 +6918,7 @@
       <c r="BW43" s="29"/>
     </row>
     <row r="44" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="64"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="14" t="s">
         <v>76</v>
       </c>
@@ -6992,7 +7007,7 @@
       <c r="BW44" s="29"/>
     </row>
     <row r="45" spans="1:75" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="64"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="14" t="s">
         <v>77</v>
       </c>
@@ -7081,7 +7096,7 @@
       <c r="BW45" s="29"/>
     </row>
     <row r="46" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="64"/>
+      <c r="A46" s="49"/>
       <c r="B46" s="14" t="s">
         <v>78</v>
       </c>
@@ -7170,7 +7185,7 @@
       <c r="BW46" s="29"/>
     </row>
     <row r="47" spans="1:75" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="64"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="14" t="s">
         <v>79</v>
       </c>
@@ -7262,7 +7277,7 @@
       <c r="A48" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="44" t="s">
         <v>108</v>
       </c>
       <c r="C48" s="14">
@@ -7301,14 +7316,10 @@
       <c r="AD48" s="29"/>
       <c r="AE48" s="29"/>
       <c r="AF48" s="29"/>
-      <c r="AG48" s="29">
-        <v>2</v>
-      </c>
+      <c r="AG48" s="29"/>
       <c r="AH48" s="24"/>
       <c r="AI48" s="25"/>
-      <c r="AJ48" s="25">
-        <v>2</v>
-      </c>
+      <c r="AJ48" s="25"/>
       <c r="AK48" s="26"/>
       <c r="AL48" s="26"/>
       <c r="AM48" s="26"/>
@@ -7342,11 +7353,15 @@
       <c r="BO48" s="26"/>
       <c r="BP48" s="27"/>
       <c r="BQ48" s="28"/>
-      <c r="BR48" s="29"/>
+      <c r="BR48" s="29">
+        <v>2</v>
+      </c>
       <c r="BS48" s="29"/>
       <c r="BT48" s="29"/>
       <c r="BU48" s="29"/>
-      <c r="BV48" s="29"/>
+      <c r="BV48" s="29">
+        <v>2</v>
+      </c>
       <c r="BW48" s="29"/>
     </row>
     <row r="49" spans="1:63" ht="13.2" x14ac:dyDescent="0.25">
@@ -33065,11 +33080,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="A30:A41"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A42:A47"/>
     <mergeCell ref="BQ1:BW1"/>
     <mergeCell ref="A6:A15"/>
     <mergeCell ref="AO1:AU1"/>
@@ -33085,6 +33095,11 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="A30:A41"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A42:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -33098,8 +33113,8 @@
   </sheetPr>
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>